<commit_message>
- Interview Litzel - Nutzungsanforderungen erweitert
</commit_message>
<xml_diff>
--- a/02_Festlegen_der_Nutzungsanforderungen/Requirementsdokument_QIS.xlsx
+++ b/02_Festlegen_der_Nutzungsanforderungen/Requirementsdokument_QIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carola\Desktop\OTH\HCI\HCI_OTH_APP\02_Festlegen_der_Nutzungsanforderungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FA7B629-E6FA-4D55-B396-7B72E536967E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BBF259AA-6BC2-40C5-AAAF-08BC78142779}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="15825" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="111">
   <si>
     <t>Kommentar</t>
   </si>
@@ -332,13 +332,40 @@
   </si>
   <si>
     <t>Der Nutzer muss die Prüfungen nach Studiengängen  filtern können.</t>
+  </si>
+  <si>
+    <t>2.7 Abschlussarbeiten-Eintragung</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss alle Daten zu Abschlussarbeiten  manuell eintragen können.</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss per Tastenkombination speichern können</t>
+  </si>
+  <si>
+    <t>2.8 Leistungsübersicht</t>
+  </si>
+  <si>
+    <t>2.9 Prüfungsübersicht</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss alle Daten aller Studenten einsehen könne.</t>
+  </si>
+  <si>
+    <t>2.9.1.</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss alle Prüfungen mit zugehörigen Daten einsehen können.</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss nach Studenten mittel Namen und/ oder Matrikelnr suchen können.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -404,6 +431,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -438,12 +472,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -479,8 +512,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,8 +556,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -583,14 +632,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="27" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="28">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -604,6 +650,7 @@
     <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Eingabe" xfId="27" builtinId="20"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -956,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="122" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="122" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1615,7 @@
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="29" t="s">
         <v>61</v>
       </c>
       <c r="F34" s="17" t="s">
@@ -1739,11 +1786,26 @@
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
+      <c r="C44" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
@@ -1752,37 +1814,47 @@
       <c r="J44" s="16"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+    <row r="47" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
@@ -1790,8 +1862,12 @@
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="C48" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
@@ -1800,13 +1876,15 @@
       <c r="J48" s="18"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
@@ -1814,8 +1892,12 @@
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>

</xml_diff>

<commit_message>
Added Bilder und Instruktionen/Workflow zum Test in Axure für Professoren und Student/Praktikumsverwaltung
</commit_message>
<xml_diff>
--- a/02_Festlegen_der_Nutzungsanforderungen/Requirementsdokument_QIS.xlsx
+++ b/02_Festlegen_der_Nutzungsanforderungen/Requirementsdokument_QIS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\career\study\term6\human_computer_interactions\project_oth_app\02_Festlegen_der_Nutzungsanforderungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Simon\Uni\Semester6\HCI\git\02_Festlegen_der_Nutzungsanforderungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B91B30-998C-414E-8CAB-BA8E4962CEF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5216F4-6119-45B0-9A74-6D5796C4DB0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="15825" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t>Notenansicht</t>
   </si>
   <si>
-    <t>Der Nutzer muss die Prüfungen nach Studiengängen  filtern können.</t>
-  </si>
-  <si>
     <t>2.7 Abschlussarbeiten-Eintragung</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>Der Nutzer muss alle Daten aller Studenten einsehen können.</t>
+  </si>
+  <si>
+    <t>Der Nutzer muss die Prüfungen nach Studiengängen  filtern/sortieren können.</t>
   </si>
 </sst>
 </file>
@@ -1009,16 +1009,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="122" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="122" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.1875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.875" style="1"/>
     <col min="8" max="8" width="13.125" style="1" customWidth="1"/>
@@ -1028,7 +1028,7 @@
     <col min="14" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1040,7 +1040,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1052,7 +1052,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.5">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1080,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1106,7 +1106,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1118,7 +1118,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.5">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
@@ -1129,10 +1129,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>1</v>
@@ -1145,7 +1145,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>37</v>
@@ -1159,7 +1159,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="12"/>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -1174,7 +1174,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B11" s="12"/>
       <c r="C11" s="2" t="s">
         <v>36</v>
@@ -1189,7 +1189,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.5">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1206,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
@@ -1226,7 +1226,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B14" s="12"/>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -1247,7 +1247,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>13</v>
@@ -1263,7 +1263,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B16" s="12"/>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1284,7 +1284,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B17" s="12"/>
       <c r="C17" s="2" t="s">
         <v>9</v>
@@ -1305,7 +1305,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B18" s="12"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1326,7 +1326,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>22</v>
@@ -1342,7 +1342,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B20" s="12"/>
       <c r="C20" s="16" t="s">
         <v>18</v>
@@ -1363,7 +1363,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B21" s="12"/>
       <c r="C21" s="16" t="s">
         <v>19</v>
@@ -1384,7 +1384,7 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B22" s="12"/>
       <c r="C22" s="16" t="s">
         <v>20</v>
@@ -1405,7 +1405,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B23" s="12"/>
       <c r="C23" s="16" t="s">
         <v>24</v>
@@ -1426,7 +1426,7 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="C24" s="16" t="s">
         <v>25</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
       <c r="C25" s="16" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
       <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
         <v>30</v>
@@ -1493,7 +1493,7 @@
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="2"/>
       <c r="B28" s="12"/>
       <c r="C28" s="16" t="s">
@@ -1515,7 +1515,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="2"/>
       <c r="B29" s="12"/>
       <c r="C29" s="16" t="s">
@@ -1537,7 +1537,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A30" s="2"/>
       <c r="B30" s="12"/>
       <c r="C30" s="16" t="s">
@@ -1559,7 +1559,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A31" s="2"/>
       <c r="B31" s="12"/>
       <c r="C31" s="16" t="s">
@@ -1581,7 +1581,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>31</v>
@@ -1597,7 +1597,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="2"/>
       <c r="B33" s="12"/>
       <c r="C33" s="2" t="s">
@@ -1619,7 +1619,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>67</v>
@@ -1639,7 +1639,7 @@
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -1651,7 +1651,7 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>48</v>
@@ -1665,7 +1665,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
     </row>
-    <row r="37" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16" t="s">
@@ -1687,7 +1687,7 @@
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18" t="s">
@@ -1709,14 +1709,14 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18" t="s">
         <v>53</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>40</v>
@@ -1731,7 +1731,7 @@
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18" t="s">
@@ -1753,7 +1753,7 @@
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18" t="s">
@@ -1775,7 +1775,7 @@
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18" t="s">
@@ -1797,10 +1797,10 @@
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -1808,14 +1808,14 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16" t="s">
         <v>49</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -1824,14 +1824,14 @@
       <c r="I44" s="16"/>
       <c r="J44" s="16"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -1840,10 +1840,10 @@
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -1854,14 +1854,14 @@
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16" t="s">
         <v>49</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
@@ -1870,14 +1870,14 @@
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
@@ -1886,10 +1886,10 @@
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -1900,14 +1900,14 @@
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
@@ -1916,7 +1916,7 @@
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -1928,7 +1928,7 @@
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -1940,103 +1940,103 @@
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B53" s="14"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B54" s="14"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B55" s="14"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B56" s="14"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B57" s="14"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B58" s="14"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B59" s="14"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B60" s="14"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B61" s="14"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B62" s="14"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B63" s="14"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B64" s="14"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B65" s="14"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B66" s="14"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B67" s="14"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B68" s="14"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B69" s="14"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B70" s="14"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B71" s="14"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B72" s="14"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B73" s="14"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B74" s="14"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B75" s="14"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B76" s="14"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B78" s="14"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B79" s="14"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B80" s="14"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B81" s="14"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B82" s="14"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B83" s="14"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B84" s="14"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B85" s="14"/>
     </row>
   </sheetData>
@@ -2058,7 +2058,7 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
@@ -2069,7 +2069,7 @@
     <col min="8" max="8" width="37.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>88</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B2" s="20" t="s">
         <v>68</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B3" s="20" t="s">
         <v>85</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B4" s="20" t="s">
         <v>90</v>
       </c>
@@ -2125,110 +2125,110 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B5" s="20"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B6" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B7" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B8" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B9" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="47.25" x14ac:dyDescent="0.5">
       <c r="B10" s="23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B12" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B13" s="24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B14" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B15" s="24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B16" s="22"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B17" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B18" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B19" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B20" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B21" s="25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B22" s="25"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B23" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B24" s="25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B25" s="26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B26" s="27"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B27" s="27"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B28" s="28" t="s">
         <v>97</v>
       </c>

</xml_diff>